<commit_message>
continuando o dev da modelagem
</commit_message>
<xml_diff>
--- a/db/tabelas_ER_bd.xlsx
+++ b/db/tabelas_ER_bd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_conceitual_repairIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33141E95-7BB7-4AD1-BB7D-3DE323516F6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4966B26-69CB-43D9-9DBB-932476D1E83E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Relacionamento</t>
   </si>
@@ -196,9 +196,6 @@
     <t>possui</t>
   </si>
   <si>
-    <t>aberta por</t>
-  </si>
-  <si>
     <t>contem</t>
   </si>
   <si>
@@ -215,6 +212,12 @@
   </si>
   <si>
     <t>gera analise</t>
+  </si>
+  <si>
+    <t>aberta</t>
+  </si>
+  <si>
+    <t>gera</t>
   </si>
 </sst>
 </file>
@@ -700,22 +703,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1058,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,22 +1080,22 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="F3" s="46" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="F3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="46"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
@@ -1112,12 +1115,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="45" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="19" t="s">
@@ -1125,81 +1128,81 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="44"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="29"/>
       <c r="C9" s="1"/>
-      <c r="F9" s="44"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="F11" s="44"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="F12" s="44"/>
+      <c r="F12" s="46"/>
       <c r="G12" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="F13" s="45"/>
+      <c r="F13" s="47"/>
       <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="48" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -1207,107 +1210,107 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="44"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="44"/>
+        <v>63</v>
+      </c>
+      <c r="F16" s="46"/>
       <c r="G16" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="44"/>
+        <v>57</v>
+      </c>
+      <c r="F17" s="46"/>
       <c r="G17" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="44"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="29"/>
       <c r="C19" s="1"/>
-      <c r="F19" s="44"/>
+      <c r="F19" s="46"/>
       <c r="G19" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="29"/>
       <c r="C20" s="1"/>
-      <c r="F20" s="44"/>
+      <c r="F20" s="46"/>
       <c r="G20" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="29"/>
       <c r="C21" s="1"/>
-      <c r="F21" s="44"/>
+      <c r="F21" s="46"/>
       <c r="G21" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="29"/>
       <c r="C22" s="1"/>
-      <c r="F22" s="44"/>
+      <c r="F22" s="46"/>
       <c r="G22" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="F23" s="45"/>
+      <c r="F23" s="47"/>
       <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="48" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="22" t="s">
@@ -1315,68 +1318,68 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="F25" s="44"/>
+      <c r="F25" s="46"/>
       <c r="G25" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="44"/>
+        <v>57</v>
+      </c>
+      <c r="F26" s="46"/>
       <c r="G26" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="F27" s="44"/>
+      <c r="F27" s="46"/>
       <c r="G27" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="F28" s="44"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="F29" s="44"/>
+      <c r="F29" s="46"/>
       <c r="G29" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="45"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="29"/>
       <c r="C30" s="1"/>
-      <c r="F30" s="45"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
-      <c r="F31" s="43" t="s">
+      <c r="F31" s="48" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="22" t="s">
@@ -1384,69 +1387,73 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="17" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="44"/>
+        <v>63</v>
+      </c>
+      <c r="F32" s="46"/>
       <c r="G32" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" s="44"/>
+        <v>58</v>
+      </c>
+      <c r="F33" s="46"/>
       <c r="G33" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="46"/>
       <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="F34" s="46"/>
       <c r="G34" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="44"/>
+        <v>60</v>
+      </c>
+      <c r="F35" s="46"/>
       <c r="G35" s="19"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="1"/>
-      <c r="F36" s="45"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="47"/>
       <c r="G36" s="24"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
-      <c r="F37" s="43" t="s">
+      <c r="F37" s="48" t="s">
         <v>12</v>
       </c>
       <c r="G37" s="22" t="s">
@@ -1454,48 +1461,48 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
+      <c r="A38" s="46"/>
       <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F38" s="44"/>
+        <v>60</v>
+      </c>
+      <c r="F38" s="46"/>
       <c r="G38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="F39" s="44"/>
+      <c r="F39" s="46"/>
       <c r="G39" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="F40" s="44"/>
+      <c r="F40" s="46"/>
       <c r="G40" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="F41" s="44"/>
+      <c r="F41" s="46"/>
       <c r="G41" s="19"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="45"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="31"/>
       <c r="C42" s="2"/>
-      <c r="F42" s="45"/>
+      <c r="F42" s="47"/>
       <c r="G42" s="25"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1526,7 +1533,7 @@
         <v>11</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="27" t="s">
@@ -1539,7 +1546,7 @@
         <v>55</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="27" t="s">
@@ -1599,7 +1606,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="27" t="s">
@@ -1666,7 +1673,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F59" s="41"/>
       <c r="G59" s="27" t="s">
@@ -1679,7 +1686,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F60" s="41"/>
       <c r="G60" s="27" t="s">
@@ -1688,8 +1695,12 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="F61" s="41"/>
       <c r="G61" s="27" t="s">
         <v>46</v>
@@ -1787,12 +1798,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="F51:F57"/>
-    <mergeCell ref="F58:F63"/>
-    <mergeCell ref="F64:F69"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="F31:F36"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="F43:F50"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="A6:A13"/>
@@ -1801,12 +1812,12 @@
     <mergeCell ref="F6:F13"/>
     <mergeCell ref="F14:F23"/>
     <mergeCell ref="F24:F30"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="F31:F36"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="F43:F50"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="F51:F57"/>
+    <mergeCell ref="F58:F63"/>
+    <mergeCell ref="F64:F69"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1828,14 +1839,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="43"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
@@ -1846,127 +1857,127 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="10"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="11"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="10"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
+      <c r="A29" s="48"/>
       <c r="B29" s="11"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="46"/>
       <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="46"/>
       <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="45"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alteração da cor das tabelas.
</commit_message>
<xml_diff>
--- a/db/tabelas_ER_bd.xlsx
+++ b/db/tabelas_ER_bd.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\4DSN_val\BD_conceitual_repairIQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Documents\RepairIQ\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF0BAF-C158-4B44-A8B8-C1E1B2E40855}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0CF0CF-49BF-498B-AED4-2DEF88BBD429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,7 +192,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +211,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -536,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -574,108 +580,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -684,19 +598,123 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1039,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,655 +1071,655 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="F3" s="28" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="F3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="28"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="59"/>
+      <c r="G7" s="33" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="13" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="33" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="13"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="13" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="33"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="14"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="13" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="33" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="14"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="13" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="33" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="14"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="15"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="54"/>
+      <c r="G15" s="55" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="40" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="17" t="s">
+      <c r="F16" s="54"/>
+      <c r="G16" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="40" t="s">
+      <c r="A17" s="31"/>
+      <c r="B17" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="17" t="s">
+      <c r="F17" s="54"/>
+      <c r="G17" s="55" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="38" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="54"/>
+      <c r="G18" s="55" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="13"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="31"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="33"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="43"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="13"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="31"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="33"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="43"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="13"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="31"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="33"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="43"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="13"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="31"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="33"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="43"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="15"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="41"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="13"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="13" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="39"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="13" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="35"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="33" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="13"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="13"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="13"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="13"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="13"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="13"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="15"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="17"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="41"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="55"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="33" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="35"/>
-      <c r="G32" s="13" t="s">
+      <c r="F32" s="54"/>
+      <c r="G32" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="35"/>
-      <c r="G33" s="13" t="s">
+      <c r="F33" s="54"/>
+      <c r="G33" s="33" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="13"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="33"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="33"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="13"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="33"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="24"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="17"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="47"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="55"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="33" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="40" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="35"/>
-      <c r="G38" s="13" t="s">
+      <c r="F38" s="54"/>
+      <c r="G38" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="13"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="13" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="33" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="40"/>
-      <c r="C40" s="13"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="13"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="33"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="13"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="13"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="33"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
-      <c r="B42" s="41"/>
-      <c r="C42" s="15"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="17"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="41"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="G43" s="55" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="52" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="53" t="s">
+      <c r="C44" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="17" t="s">
+      <c r="F44" s="54"/>
+      <c r="G44" s="55" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="39"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="17" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="35"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="55" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="39"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="17" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="35"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="55" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="53"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="17"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="51"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="55"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="13"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="17"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="33"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="55"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="55"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="17"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="53"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="55"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="15"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="17"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="41"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="55"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F51" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="G51" s="55" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="39"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="17" t="s">
+      <c r="A52" s="31"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="35"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="55" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="53"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="17" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="55" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="52"/>
-      <c r="C54" s="53"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="17"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="55"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="53"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="17"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="55"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="54"/>
-      <c r="C56" s="55"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="17"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="53"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="55"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="15"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="17"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="41"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="55"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="51" t="s">
+      <c r="B58" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F58" s="35" t="s">
+      <c r="F58" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="G58" s="17" t="s">
+      <c r="G58" s="55" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="52"/>
-      <c r="C59" s="53"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="17" t="s">
+      <c r="A59" s="31"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="51"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="55" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="52"/>
-      <c r="C60" s="53"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="17"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="51"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="55"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="39"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="17"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="35"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="55"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
-      <c r="B62" s="52"/>
-      <c r="C62" s="53"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="17"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+      <c r="F62" s="54"/>
+      <c r="G62" s="55"/>
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="24"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="15"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="17"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="45"/>
+      <c r="C63" s="41"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="55"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="51" t="s">
+      <c r="B64" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F64" s="35" t="s">
+      <c r="F64" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G64" s="55" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="52"/>
-      <c r="C65" s="53"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="17"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="51"/>
+      <c r="F65" s="54"/>
+      <c r="G65" s="55"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="53"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="17"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="51"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="55"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="53"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="17"/>
+      <c r="A67" s="31"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="51"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="55"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-      <c r="B68" s="52"/>
-      <c r="C68" s="53"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="17"/>
+      <c r="A68" s="31"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="51"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="55"/>
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="24"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="15"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="18"/>
+      <c r="A69" s="39"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="41"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="57"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G70"/>
@@ -1723,12 +1741,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A64:A69"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="F51:F57"/>
-    <mergeCell ref="F58:F63"/>
-    <mergeCell ref="F64:F69"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="F31:F36"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="F43:F50"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="F3:G4"/>
     <mergeCell ref="A6:A13"/>
@@ -1737,12 +1755,12 @@
     <mergeCell ref="F6:F13"/>
     <mergeCell ref="F14:F23"/>
     <mergeCell ref="F24:F30"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="F31:F36"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="F43:F50"/>
+    <mergeCell ref="A64:A69"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="F51:F57"/>
+    <mergeCell ref="F58:F63"/>
+    <mergeCell ref="F64:F69"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1764,193 +1782,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="1"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="1"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="8"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="9"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="9"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="9"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="9"/>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="10"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="8"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="20"/>
       <c r="B42" s="9"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="11"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="11"/>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="10"/>
     </row>
   </sheetData>

</xml_diff>